<commit_message>
mudanças no prompt e teste na saida
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Modelo          </t>
+          <t xml:space="preserve">Modelo      </t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -461,123 +461,863 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">CPF              </t>
+          <t xml:space="preserve">CPF                </t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">RG            </t>
+          <t xml:space="preserve">RG                 </t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">QYF-5J92 </t>
+          <t xml:space="preserve">JGN-1239 </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Onix            </t>
+          <t xml:space="preserve">Civic       </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chevrolet </t>
+          <t xml:space="preserve">Honda    </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Branco   </t>
+          <t xml:space="preserve">Prata    </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">GILVEANO COTA            </t>
+          <t xml:space="preserve">Gilveano Cota            </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">020.856.860-36 </t>
+          <t xml:space="preserve">020.856.860-36    </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1092477941   </t>
+          <t xml:space="preserve">1092477941 SSP RS </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">PRQ8F00  </t>
+          <t xml:space="preserve">PAE-1239 </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Discovery Sport </t>
+          <t xml:space="preserve">HB20S       </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Land Rover</t>
+          <t xml:space="preserve">Hyundai  </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Azul Escuro</t>
+          <t xml:space="preserve">Prata    </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">ISAC SOARES CAMARA JUNIOR </t>
+          <t xml:space="preserve">Isaac Soares Câmara Júnior </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">016.016.291-25 </t>
+          <t xml:space="preserve">016.016.291-25    </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">2617795      </t>
+          <t xml:space="preserve">2617795 SSP DF    </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">IMPERIAL </t>
+          <t xml:space="preserve">RBU2C69  </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mobi            </t>
+          <t xml:space="preserve">Onix        </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t xml:space="preserve">Chevrolet </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Branco   </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rafaela Kuhn Valandro     </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">016.718.370-29    </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1077638623 SJS/RS </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IDZ-5977 </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Omega       </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chevrolet </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Preto    </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lúcio José Assis da Silva </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3332350           </t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilegível          </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DGJ-2659 </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uno Mille   </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t xml:space="preserve">Fiat     </t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinza    </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thiago Santos Barros      </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">036.055.841-01    </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilegível          </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RUK2E39  </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mobi        </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fiat     </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinza    </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solange Maria da Silva    </t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">668.200.573-34    </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1545861 SSP PI    </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilegível </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grand Cherokee </t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jeep    </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t xml:space="preserve">Branco   </t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RAFAELA KUHN VALANDRO    </t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">016.718.370-29 </t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1077638623   </t>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rafael Ramos Peres        </t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">091.058.389-75    </t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12430705-8 SESP   </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilegível </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creta       </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hyundai  </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Preto    </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matheus Souza Roque da Silva </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">020.494.546-19    </t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MG18795190 SSP    </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JEP-9909 </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Escort      </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ford     </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Preto    </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ottimar dos Reis Saffier </t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">726.944.757-87    </t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">05936131DETRANRJ </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PBF5129  </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Argo        </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fiat     </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prata    </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Romildo de Oliveira Porto Júnior </t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">011.728.465-37    </t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1441805 SSP       </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PAH1E54  </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KA          </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ford     </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Branco   </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adilson Hamilton de Arruda </t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">466.264.681-20    </t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">462772           </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PBI7069  </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ranger      </t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ford     </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinza    </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fábio Chagas Theophilo   </t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilegível          </t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilegível          </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REQ5D29  </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tiguan Allspace </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Volkswagen </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Branco   </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Benedito Sousa Alves     </t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">054.739.813-11    </t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">036102752008-6 GE </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KDS9X69  </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mobi        </t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fiat     </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinza    </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diogo Fernandez Canabal Alves </t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">219.634.508-33    </t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3235320 SSP/SP    </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FGR-8868 </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Q3          </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Audi     </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Preto    </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mauricio Carvalho Barroso </t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">075.253.107-77    </t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1081919821PRJ    </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OLV3G67  </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Palio       </t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fiat     </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prata    </t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vitor Moisés da Cunha Silva </t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">077.227.653-60    </t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4138680 SSP PI    </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JIW-0597 </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fit         </t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honda    </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prata    </t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">José Aparecido Ribeiro   </t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">061.969.978-74    </t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">16569506 SSP/SP    </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SSU3186  </t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kwid        </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Renault  </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Branco   </t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pedro Marini Lopes       </t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">781.649.338-91    </t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">76692218 SSP/SP    </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JHK-1329 </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Corsa Classic </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chevrolet </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Preto    </t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wagner Torres Pires de Carvalho </t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">714.085.849-72    </t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">22862249 SSP/SP    </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QYF-5J92 </t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prisma Joy  </t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chevrolet </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Branco   </t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Euler Fernando Grandolpho </t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">161.639.748-30    </t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">102551175 SSP/SP    </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GKJ3B09  </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chevette    </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chevrolet </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinza    </t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Afraim Freires dos Santos </t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">766.879.712-04    </t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">415617 SSP AC     </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SGY1A99  </t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Commander   </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jeep    </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prata    </t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alan Machado Correa      </t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">125.974.457-47    </t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ilegível          </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRQ8F00  </t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Discovery Sport </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Land Rover </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Azul Escuro </t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Luiz Fernando Ramos      </t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">118.453.886-74    </t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MG18846936 SSP    </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mudança da função verbose para saber onde o codigo esta no momento e o que esta levando tempo.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -436,37 +436,37 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Placa    </t>
+          <t xml:space="preserve">Placa </t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Modelo      </t>
+          <t xml:space="preserve">Modelo </t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Marca    </t>
+          <t xml:space="preserve">Marca </t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cor      </t>
+          <t xml:space="preserve">Cor </t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nome                      </t>
+          <t xml:space="preserve">Nome </t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">CPF                </t>
+          <t xml:space="preserve">CPF </t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">RG                 </t>
+          <t xml:space="preserve">RG </t>
         </is>
       </c>
     </row>
@@ -478,32 +478,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Civic       </t>
+          <t xml:space="preserve">Civic </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Honda    </t>
+          <t xml:space="preserve">Honda </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prata    </t>
+          <t xml:space="preserve">Prata </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gilveano Cota            </t>
+          <t xml:space="preserve">Gilveano Cota </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">020.856.860-36    </t>
+          <t xml:space="preserve">020.856.860-36 </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1092477941 SSP RS </t>
+          <t xml:space="preserve">1092477941 SSP/RS </t>
         </is>
       </c>
     </row>
@@ -515,17 +515,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">HB20S       </t>
+          <t xml:space="preserve">HB20S </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hyundai  </t>
+          <t xml:space="preserve">Hyundai </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prata    </t>
+          <t xml:space="preserve">Prata </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,24 +535,24 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">016.016.291-25    </t>
+          <t xml:space="preserve">016.016.291-25 </t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">2617795 SSP DF    </t>
+          <t xml:space="preserve">2617795 SSP/DF </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">RBU2C69  </t>
+          <t xml:space="preserve">RBU2C69 </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Onix        </t>
+          <t xml:space="preserve">Onix </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -562,22 +562,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Branco   </t>
+          <t xml:space="preserve">Branco </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rafaela Kuhn Valandro     </t>
+          <t xml:space="preserve">Rafaela Kuhn Valandro </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">016.718.370-29    </t>
+          <t xml:space="preserve">016.718.370-29 </t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1077638623 SJS/RS </t>
+          <t xml:space="preserve">1077638623 SJS/FI RS </t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Omega       </t>
+          <t xml:space="preserve">Omega </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -599,22 +599,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Preto    </t>
+          <t xml:space="preserve">Preto </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lúcio José Assis da Silva </t>
+          <t xml:space="preserve">Lucio José Assis da Silva </t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">3332350           </t>
+          <t xml:space="preserve">054.172.355-39 </t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ilegível          </t>
+          <t xml:space="preserve">33323500 SSP/SE </t>
         </is>
       </c>
     </row>
@@ -626,78 +626,74 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Uno Mille   </t>
+          <t xml:space="preserve">Uno </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fiat     </t>
+          <t xml:space="preserve">Fiat </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cinza    </t>
+          <t xml:space="preserve">Cinza Escuro </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Thiago Santos Barros      </t>
+          <t xml:space="preserve">Thiago Santos Barros </t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">036.055.841-01    </t>
+          <t xml:space="preserve">036.055.841-01 </t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ilegível          </t>
+          <t xml:space="preserve">Ilegível </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">RUK2E39  </t>
+          <t xml:space="preserve">RUK2E39 </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mobi        </t>
+          <t xml:space="preserve">Mobi </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fiat     </t>
+          <t xml:space="preserve">Fiat </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cinza    </t>
+          <t xml:space="preserve">Cinza Escuro </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Solange Maria da Silva    </t>
+          <t xml:space="preserve">Solange Maria da Silva </t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">668.200.573-34    </t>
+          <t xml:space="preserve">668.200.573-34 </t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">1545861 SSP PI    </t>
+          <t xml:space="preserve">1545861 SSP/PI </t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ilegível </t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
           <t xml:space="preserve">Grand Cherokee </t>
@@ -705,49 +701,45 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jeep    </t>
+          <t xml:space="preserve">Jeep </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Branco   </t>
+          <t xml:space="preserve">Branco </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rafael Ramos Peres        </t>
+          <t xml:space="preserve">Rafael Ramos Peres </t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">091.058.389-75    </t>
+          <t xml:space="preserve">091.058.389-75 </t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve">12430705-8 SESP   </t>
+          <t xml:space="preserve">12430705-8 SESP/PR </t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Ilegível </t>
-        </is>
-      </c>
+      <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Creta       </t>
+          <t xml:space="preserve">Creta </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hyundai  </t>
+          <t xml:space="preserve">Hyundai </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Preto    </t>
+          <t xml:space="preserve">Preto </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -757,12 +749,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">020.494.546-19    </t>
+          <t xml:space="preserve">020.494.546-19 </t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">MG18795190 SSP    </t>
+          <t xml:space="preserve">MG18795190 SSP/MG </t>
         </is>
       </c>
     </row>
@@ -774,27 +766,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Escort      </t>
+          <t xml:space="preserve">Escort </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ford     </t>
+          <t xml:space="preserve">Ford </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Preto    </t>
+          <t xml:space="preserve">Preto </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ottimar dos Reis Saffier </t>
+          <t xml:space="preserve">Otmar dos Reis Saffier </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">726.944.757-87    </t>
+          <t xml:space="preserve">726.944.757-87 </t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -806,22 +798,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">PBF5129  </t>
+          <t xml:space="preserve">PBF5129 </t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Argo        </t>
+          <t xml:space="preserve">Argo </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fiat     </t>
+          <t xml:space="preserve">Fiat </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prata    </t>
+          <t xml:space="preserve">Prata </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -831,34 +823,34 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">011.728.465-37    </t>
+          <t xml:space="preserve">011.728.465-37 </t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t xml:space="preserve">1441805 SSP       </t>
+          <t xml:space="preserve">1441805 SSP/SE </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">PAH1E54  </t>
+          <t xml:space="preserve">PAH1E54 </t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">KA          </t>
+          <t xml:space="preserve">Ka </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ford     </t>
+          <t xml:space="preserve">Ford </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Branco   </t>
+          <t xml:space="preserve">Branco </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -868,61 +860,61 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">466.264.681-20    </t>
+          <t xml:space="preserve">466.264.681-20 </t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve">462772           </t>
+          <t xml:space="preserve">462772 SSP/MS </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">PBI7069  </t>
+          <t xml:space="preserve">PBI-7069 </t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ranger      </t>
+          <t xml:space="preserve">Ranger </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ford     </t>
+          <t xml:space="preserve">Ford </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cinza    </t>
+          <t xml:space="preserve">Cinza Escuro </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fábio Chagas Theophilo   </t>
+          <t xml:space="preserve">Fábio Chagas Theophilo </t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ilegível          </t>
+          <t xml:space="preserve">Ilegível </t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ilegível          </t>
+          <t xml:space="preserve">Ilegível </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">REQ5D29  </t>
+          <t xml:space="preserve">REQ5D29 </t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tiguan Allspace </t>
+          <t xml:space="preserve">Tiguan </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -932,44 +924,44 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Branco   </t>
+          <t xml:space="preserve">Branco </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Benedito Sousa Alves     </t>
+          <t xml:space="preserve">Benedito Sousa Alves </t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve">054.739.813-11    </t>
+          <t xml:space="preserve">054.739.813-6 </t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t xml:space="preserve">036102752008-6 GE </t>
+          <t xml:space="preserve">036102752008-6 GE/UF/MA </t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">KDS9X69  </t>
+          <t xml:space="preserve">KDS9X69 </t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mobi        </t>
+          <t xml:space="preserve">Mobi </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fiat     </t>
+          <t xml:space="preserve">Fiat </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cinza    </t>
+          <t xml:space="preserve">Cinza Escuro </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -979,12 +971,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve">219.634.508-33    </t>
+          <t xml:space="preserve">219.634.508-33 </t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">3235320 SSP/SP    </t>
+          <t xml:space="preserve">3235320 SSP/SP </t>
         </is>
       </c>
     </row>
@@ -996,54 +988,54 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Q3          </t>
+          <t xml:space="preserve">Q3 </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Audi     </t>
+          <t xml:space="preserve">Audi </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Preto    </t>
+          <t xml:space="preserve">Preto </t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mauricio Carvalho Barroso </t>
+          <t xml:space="preserve">Mauricio Carvalho Barros </t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve">075.253.107-77    </t>
+          <t xml:space="preserve">075.253.107-77 </t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">1081919821PRJ    </t>
+          <t xml:space="preserve">1081919821/PRJ </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">OLV3G67  </t>
+          <t xml:space="preserve">OLV3G67 </t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Palio       </t>
+          <t xml:space="preserve">Palio </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fiat     </t>
+          <t xml:space="preserve">Fiat </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prata    </t>
+          <t xml:space="preserve">Prata </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1053,12 +1045,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve">077.227.653-60    </t>
+          <t xml:space="preserve">077.227.653-60 </t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t xml:space="preserve">4138680 SSP PI    </t>
+          <t xml:space="preserve">4138680 SSP/PI </t>
         </is>
       </c>
     </row>
@@ -1070,69 +1062,69 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fit         </t>
+          <t xml:space="preserve">Fit </t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Honda    </t>
+          <t xml:space="preserve">Honda </t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prata    </t>
+          <t xml:space="preserve">Prata </t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">José Aparecido Ribeiro   </t>
+          <t xml:space="preserve">José Aparecido Ribeiro </t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">061.969.978-74    </t>
+          <t xml:space="preserve">061.969.978-74 </t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t xml:space="preserve">16569506 SSP/SP    </t>
+          <t xml:space="preserve">16569506 SSP/SP </t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">SSU3186  </t>
+          <t xml:space="preserve">SSU3186 </t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kwid        </t>
+          <t xml:space="preserve">Kwid </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Renault  </t>
+          <t xml:space="preserve">Renault </t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Branco   </t>
+          <t xml:space="preserve">Branco </t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pedro Marini Lopes       </t>
+          <t xml:space="preserve">Pedro Marini Lopes </t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">781.649.338-91    </t>
+          <t xml:space="preserve">781.649.338-91 </t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t xml:space="preserve">76692218 SSP/SP    </t>
+          <t xml:space="preserve">76632218 SSP/SP </t>
         </is>
       </c>
     </row>
@@ -1154,7 +1146,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Preto    </t>
+          <t xml:space="preserve">Preto </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1164,12 +1156,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve">714.085.849-72    </t>
+          <t xml:space="preserve">714.085.849-72 </t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t xml:space="preserve">22862249 SSP/SP    </t>
+          <t xml:space="preserve">22862249 SSP/SP </t>
         </is>
       </c>
     </row>
@@ -1181,7 +1173,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prisma Joy  </t>
+          <t xml:space="preserve">Onix </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1191,7 +1183,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Branco   </t>
+          <t xml:space="preserve">Branco </t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1201,24 +1193,24 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve">161.639.748-30    </t>
+          <t xml:space="preserve">161.639.748-30 </t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">102551175 SSP/SP    </t>
+          <t xml:space="preserve">10255175 SSP/SP </t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">GKJ3B09  </t>
+          <t xml:space="preserve">GKJ3B09 </t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chevette    </t>
+          <t xml:space="preserve">Chevette </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1228,7 +1220,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cinza    </t>
+          <t xml:space="preserve">Cinza </t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1238,56 +1230,56 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve">766.879.712-04    </t>
+          <t xml:space="preserve">766.879.712-04 </t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t xml:space="preserve">415617 SSP AC     </t>
+          <t xml:space="preserve">415617 SSP/AC </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">SGY1A99  </t>
+          <t xml:space="preserve">SGY1A99 </t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Commander   </t>
+          <t xml:space="preserve">Commander </t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jeep    </t>
+          <t xml:space="preserve">Jeep </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prata    </t>
+          <t xml:space="preserve">Prata </t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alan Machado Correa      </t>
+          <t xml:space="preserve">Alan Machado Correa </t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">125.974.457-47    </t>
+          <t xml:space="preserve">125.974.457-47 </t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ilegível          </t>
+          <t xml:space="preserve">20817030DETRANRJ </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">PRQ8F00  </t>
+          <t xml:space="preserve">PRQ8F00 </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1307,17 +1299,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Luiz Fernando Ramos      </t>
+          <t xml:space="preserve">Luiz Fernando Ramos </t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve">118.453.886-74    </t>
+          <t xml:space="preserve">118.453.886-74 </t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t xml:space="preserve">MG18846936 SSP    </t>
+          <t xml:space="preserve">MG18846936 SSP </t>
         </is>
       </c>
     </row>

</xml_diff>